<commit_message>
Commit before implementing newly designed levels
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Mechanics</t>
   </si>
@@ -152,6 +152,51 @@
   </si>
   <si>
     <t>2 wood</t>
+  </si>
+  <si>
+    <t>octopi part</t>
+  </si>
+  <si>
+    <t>time potion</t>
+  </si>
+  <si>
+    <t>octopi part*2</t>
+  </si>
+  <si>
+    <t>void shard</t>
+  </si>
+  <si>
+    <t>Fire dragon</t>
+  </si>
+  <si>
+    <t>fire shade</t>
+  </si>
+  <si>
+    <t>fire sword</t>
+  </si>
+  <si>
+    <t>fire shade + steel</t>
+  </si>
+  <si>
+    <t>1 void enemy</t>
+  </si>
+  <si>
+    <t>3 fire imp</t>
+  </si>
+  <si>
+    <t>fire imps</t>
+  </si>
+  <si>
+    <t>steel + fire shade</t>
+  </si>
+  <si>
+    <t>2 player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron </t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -255,11 +300,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -570,56 +614,61 @@
   <dimension ref="A1:O482"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
-    <col min="2" max="6" width="13.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="4" customWidth="1"/>
-    <col min="10" max="14" width="13.7109375" style="6" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="3" customWidth="1"/>
+    <col min="2" max="6" width="13.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="3" customWidth="1"/>
+    <col min="10" max="12" width="13.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="I1" s="2"/>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -627,2644 +676,2743 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>20</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>60</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>20</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>20</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>40</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="L5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>17</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="L6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>30</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="N7" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>20</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>35</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="N8" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>15</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="N9" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>15</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>40</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>60</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>30</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>20</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>40</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>20</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="H14" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="G15" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
+        <v>40</v>
+      </c>
+      <c r="C16" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="G16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="C17" s="5">
+        <v>30</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="D18" s="5">
+        <v>13</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="C19" s="5">
+        <v>25</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="D20" s="5">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="D21" s="5">
+        <v>20</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="D22" s="5">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="C23" s="5">
+        <v>40</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="E24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="B28" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="A88" s="3">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="A90" s="3">
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="A91" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="A92" s="3">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="A95" s="3">
         <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+      <c r="A96" s="3">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
+      <c r="A97" s="3">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+      <c r="A98" s="3">
         <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="A99" s="3">
         <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+      <c r="A100" s="3">
         <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="A101" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="A102" s="3">
         <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+      <c r="A103" s="3">
         <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="A104" s="3">
         <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
+      <c r="A105" s="3">
         <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+      <c r="A106" s="3">
         <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+      <c r="A107" s="3">
         <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+      <c r="A108" s="3">
         <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
+      <c r="A109" s="3">
         <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+      <c r="A110" s="3">
         <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="A111" s="3">
         <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+      <c r="A112" s="3">
         <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="4">
+      <c r="A113" s="3">
         <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
+      <c r="A114" s="3">
         <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
+      <c r="A115" s="3">
         <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+      <c r="A116" s="3">
         <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="A117" s="3">
         <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
+      <c r="A118" s="3">
         <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+      <c r="A119" s="3">
         <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
+      <c r="A120" s="3">
         <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
+      <c r="A121" s="3">
         <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
+      <c r="A122" s="3">
         <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
+      <c r="A123" s="3">
         <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
+      <c r="A124" s="3">
         <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
+      <c r="A125" s="3">
         <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
+      <c r="A126" s="3">
         <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
+      <c r="A127" s="3">
         <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+      <c r="A128" s="3">
         <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
+      <c r="A129" s="3">
         <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="A130" s="3">
         <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="A131" s="3">
         <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="A132" s="3">
         <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+      <c r="A133" s="3">
         <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+      <c r="A134" s="3">
         <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+      <c r="A135" s="3">
         <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="A136" s="3">
         <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
+      <c r="A137" s="3">
         <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="A138" s="3">
         <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+      <c r="A139" s="3">
         <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
+      <c r="A140" s="3">
         <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
+      <c r="A141" s="3">
         <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="4">
+      <c r="A142" s="3">
         <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="A143" s="3">
         <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="4">
+      <c r="A144" s="3">
         <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="4">
+      <c r="A145" s="3">
         <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="A146" s="3">
         <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="4">
+      <c r="A147" s="3">
         <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="4">
+      <c r="A148" s="3">
         <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="4">
+      <c r="A149" s="3">
         <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="4">
+      <c r="A150" s="3">
         <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="4">
+      <c r="A151" s="3">
         <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="4">
+      <c r="A152" s="3">
         <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="4">
+      <c r="A153" s="3">
         <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="4">
+      <c r="A154" s="3">
         <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="4">
+      <c r="A155" s="3">
         <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="4">
+      <c r="A156" s="3">
         <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="4">
+      <c r="A157" s="3">
         <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="4">
+      <c r="A158" s="3">
         <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="4">
+      <c r="A159" s="3">
         <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="4">
+      <c r="A160" s="3">
         <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="4">
+      <c r="A161" s="3">
         <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="4">
+      <c r="A162" s="3">
         <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="4">
+      <c r="A163" s="3">
         <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="4">
+      <c r="A164" s="3">
         <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="4">
+      <c r="A165" s="3">
         <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="4">
+      <c r="A166" s="3">
         <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="4">
+      <c r="A167" s="3">
         <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4">
+      <c r="A168" s="3">
         <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="4">
+      <c r="A169" s="3">
         <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="4">
+      <c r="A170" s="3">
         <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="4">
+      <c r="A171" s="3">
         <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="4">
+      <c r="A172" s="3">
         <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="4">
+      <c r="A173" s="3">
         <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="4">
+      <c r="A174" s="3">
         <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="4">
+      <c r="A175" s="3">
         <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="4">
+      <c r="A176" s="3">
         <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="4">
+      <c r="A177" s="3">
         <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="4">
+      <c r="A178" s="3">
         <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="4">
+      <c r="A179" s="3">
         <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="4">
+      <c r="A180" s="3">
         <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="4">
+      <c r="A181" s="3">
         <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="4">
+      <c r="A182" s="3">
         <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="4">
+      <c r="A183" s="3">
         <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="4">
+      <c r="A184" s="3">
         <v>183</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="4">
+      <c r="A185" s="3">
         <v>184</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4">
+      <c r="A186" s="3">
         <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="4">
+      <c r="A187" s="3">
         <v>186</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4">
+      <c r="A188" s="3">
         <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4">
+      <c r="A189" s="3">
         <v>188</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="4">
+      <c r="A190" s="3">
         <v>189</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4">
+      <c r="A191" s="3">
         <v>190</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="4">
+      <c r="A192" s="3">
         <v>191</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="4">
+      <c r="A193" s="3">
         <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="4">
+      <c r="A194" s="3">
         <v>193</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="4">
+      <c r="A195" s="3">
         <v>194</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4">
+      <c r="A196" s="3">
         <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="4">
+      <c r="A197" s="3">
         <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="4">
+      <c r="A198" s="3">
         <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="4">
+      <c r="A199" s="3">
         <v>198</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="4">
+      <c r="A200" s="3">
         <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="4">
+      <c r="A201" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="4">
+      <c r="A202" s="3">
         <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="4">
+      <c r="A203" s="3">
         <v>202</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4">
+      <c r="A204" s="3">
         <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="4">
+      <c r="A205" s="3">
         <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="4">
+      <c r="A206" s="3">
         <v>205</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="4">
+      <c r="A207" s="3">
         <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="4">
+      <c r="A208" s="3">
         <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="4">
+      <c r="A209" s="3">
         <v>208</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="4">
+      <c r="A210" s="3">
         <v>209</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="4">
+      <c r="A211" s="3">
         <v>210</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="4">
+      <c r="A212" s="3">
         <v>211</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="4">
+      <c r="A213" s="3">
         <v>212</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="4">
+      <c r="A214" s="3">
         <v>213</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="4">
+      <c r="A215" s="3">
         <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="4">
+      <c r="A216" s="3">
         <v>215</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="4">
+      <c r="A217" s="3">
         <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="4">
+      <c r="A218" s="3">
         <v>217</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="4">
+      <c r="A219" s="3">
         <v>218</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="4">
+      <c r="A220" s="3">
         <v>219</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" s="4">
+      <c r="A221" s="3">
         <v>220</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="4">
+      <c r="A222" s="3">
         <v>221</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="4">
+      <c r="A223" s="3">
         <v>222</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="4">
+      <c r="A224" s="3">
         <v>223</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="4">
+      <c r="A225" s="3">
         <v>224</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="4">
+      <c r="A226" s="3">
         <v>225</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="4">
+      <c r="A227" s="3">
         <v>226</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="4">
+      <c r="A228" s="3">
         <v>227</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="4">
+      <c r="A229" s="3">
         <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="4">
+      <c r="A230" s="3">
         <v>229</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="4">
+      <c r="A231" s="3">
         <v>230</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="4">
+      <c r="A232" s="3">
         <v>231</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="4">
+      <c r="A233" s="3">
         <v>232</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="4">
+      <c r="A234" s="3">
         <v>233</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="4">
+      <c r="A235" s="3">
         <v>234</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="4">
+      <c r="A236" s="3">
         <v>235</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="4">
+      <c r="A237" s="3">
         <v>236</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="4">
+      <c r="A238" s="3">
         <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="4">
+      <c r="A239" s="3">
         <v>238</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="4">
+      <c r="A240" s="3">
         <v>239</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="4">
+      <c r="A241" s="3">
         <v>240</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="4">
+      <c r="A242" s="3">
         <v>241</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="4">
+      <c r="A243" s="3">
         <v>242</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="4">
+      <c r="A244" s="3">
         <v>243</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="4">
+      <c r="A245" s="3">
         <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="4">
+      <c r="A246" s="3">
         <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="4">
+      <c r="A247" s="3">
         <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="4">
+      <c r="A248" s="3">
         <v>247</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="4">
+      <c r="A249" s="3">
         <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="4">
+      <c r="A250" s="3">
         <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="4">
+      <c r="A251" s="3">
         <v>250</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="4">
+      <c r="A252" s="3">
         <v>251</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="4">
+      <c r="A253" s="3">
         <v>252</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="4">
+      <c r="A254" s="3">
         <v>253</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="4">
+      <c r="A255" s="3">
         <v>254</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="4">
+      <c r="A256" s="3">
         <v>255</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="4">
+      <c r="A257" s="3">
         <v>256</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="4">
+      <c r="A258" s="3">
         <v>257</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="4">
+      <c r="A259" s="3">
         <v>258</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="4">
+      <c r="A260" s="3">
         <v>259</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="4">
+      <c r="A261" s="3">
         <v>260</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="4">
+      <c r="A262" s="3">
         <v>261</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="4">
+      <c r="A263" s="3">
         <v>262</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="4">
+      <c r="A264" s="3">
         <v>263</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" s="4">
+      <c r="A265" s="3">
         <v>264</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="4">
+      <c r="A266" s="3">
         <v>265</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="4">
+      <c r="A267" s="3">
         <v>266</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="4">
+      <c r="A268" s="3">
         <v>267</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="4">
+      <c r="A269" s="3">
         <v>268</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="4">
+      <c r="A270" s="3">
         <v>269</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="4">
+      <c r="A271" s="3">
         <v>270</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="4">
+      <c r="A272" s="3">
         <v>271</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="4">
+      <c r="A273" s="3">
         <v>272</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="4">
+      <c r="A274" s="3">
         <v>273</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="4">
+      <c r="A275" s="3">
         <v>274</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="4">
+      <c r="A276" s="3">
         <v>275</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="4">
+      <c r="A277" s="3">
         <v>276</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="4">
+      <c r="A278" s="3">
         <v>277</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="4">
+      <c r="A279" s="3">
         <v>278</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="4">
+      <c r="A280" s="3">
         <v>279</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="4">
+      <c r="A281" s="3">
         <v>280</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="4">
+      <c r="A282" s="3">
         <v>281</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="4">
+      <c r="A283" s="3">
         <v>282</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="4">
+      <c r="A284" s="3">
         <v>283</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="4">
+      <c r="A285" s="3">
         <v>284</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="4">
+      <c r="A286" s="3">
         <v>285</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="4">
+      <c r="A287" s="3">
         <v>286</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="4">
+      <c r="A288" s="3">
         <v>287</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="4">
+      <c r="A289" s="3">
         <v>288</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="4">
+      <c r="A290" s="3">
         <v>289</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="4">
+      <c r="A291" s="3">
         <v>290</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="4">
+      <c r="A292" s="3">
         <v>291</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="4">
+      <c r="A293" s="3">
         <v>292</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="4">
+      <c r="A294" s="3">
         <v>293</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="4">
+      <c r="A295" s="3">
         <v>294</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="4">
+      <c r="A296" s="3">
         <v>295</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="4">
+      <c r="A297" s="3">
         <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="4">
+      <c r="A298" s="3">
         <v>297</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="4">
+      <c r="A299" s="3">
         <v>298</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="4">
+      <c r="A300" s="3">
         <v>299</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="4">
+      <c r="A301" s="3">
         <v>300</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="4">
+      <c r="A302" s="3">
         <v>301</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="4">
+      <c r="A303" s="3">
         <v>302</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="4">
+      <c r="A304" s="3">
         <v>303</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="4">
+      <c r="A305" s="3">
         <v>304</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="4">
+      <c r="A306" s="3">
         <v>305</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="4">
+      <c r="A307" s="3">
         <v>306</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="4">
+      <c r="A308" s="3">
         <v>307</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="4">
+      <c r="A309" s="3">
         <v>308</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="4">
+      <c r="A310" s="3">
         <v>309</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="4">
+      <c r="A311" s="3">
         <v>310</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="4">
+      <c r="A312" s="3">
         <v>311</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="4">
+      <c r="A313" s="3">
         <v>312</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="4">
+      <c r="A314" s="3">
         <v>313</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="4">
+      <c r="A315" s="3">
         <v>314</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="4">
+      <c r="A316" s="3">
         <v>315</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="4">
+      <c r="A317" s="3">
         <v>316</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" s="4">
+      <c r="A318" s="3">
         <v>317</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="4">
+      <c r="A319" s="3">
         <v>318</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="4">
+      <c r="A320" s="3">
         <v>319</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="4">
+      <c r="A321" s="3">
         <v>320</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="4">
+      <c r="A322" s="3">
         <v>321</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="4">
+      <c r="A323" s="3">
         <v>322</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="4">
+      <c r="A324" s="3">
         <v>323</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" s="4">
+      <c r="A325" s="3">
         <v>324</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="4">
+      <c r="A326" s="3">
         <v>325</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="4">
+      <c r="A327" s="3">
         <v>326</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="4">
+      <c r="A328" s="3">
         <v>327</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="4">
+      <c r="A329" s="3">
         <v>328</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="4">
+      <c r="A330" s="3">
         <v>329</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="4">
+      <c r="A331" s="3">
         <v>330</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="4">
+      <c r="A332" s="3">
         <v>331</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" s="4">
+      <c r="A333" s="3">
         <v>332</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="4">
+      <c r="A334" s="3">
         <v>333</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="4">
+      <c r="A335" s="3">
         <v>334</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="4">
+      <c r="A336" s="3">
         <v>335</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="4">
+      <c r="A337" s="3">
         <v>336</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="4">
+      <c r="A338" s="3">
         <v>337</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="4">
+      <c r="A339" s="3">
         <v>338</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="4">
+      <c r="A340" s="3">
         <v>339</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="4">
+      <c r="A341" s="3">
         <v>340</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="4">
+      <c r="A342" s="3">
         <v>341</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="4">
+      <c r="A343" s="3">
         <v>342</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="4">
+      <c r="A344" s="3">
         <v>343</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="4">
+      <c r="A345" s="3">
         <v>344</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="4">
+      <c r="A346" s="3">
         <v>345</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="4">
+      <c r="A347" s="3">
         <v>346</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="4">
+      <c r="A348" s="3">
         <v>347</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="4">
+      <c r="A349" s="3">
         <v>348</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="4">
+      <c r="A350" s="3">
         <v>349</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="4">
+      <c r="A351" s="3">
         <v>350</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="4">
+      <c r="A352" s="3">
         <v>351</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="4">
+      <c r="A353" s="3">
         <v>352</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="4">
+      <c r="A354" s="3">
         <v>353</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" s="4">
+      <c r="A355" s="3">
         <v>354</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="4">
+      <c r="A356" s="3">
         <v>355</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="4">
+      <c r="A357" s="3">
         <v>356</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="4">
+      <c r="A358" s="3">
         <v>357</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="4">
+      <c r="A359" s="3">
         <v>358</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" s="4">
+      <c r="A360" s="3">
         <v>359</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="4">
+      <c r="A361" s="3">
         <v>360</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="4">
+      <c r="A362" s="3">
         <v>361</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="4">
+      <c r="A363" s="3">
         <v>362</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="4">
+      <c r="A364" s="3">
         <v>363</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="4">
+      <c r="A365" s="3">
         <v>364</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="4">
+      <c r="A366" s="3">
         <v>365</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="4">
+      <c r="A367" s="3">
         <v>366</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" s="4">
+      <c r="A368" s="3">
         <v>367</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="4">
+      <c r="A369" s="3">
         <v>368</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="4">
+      <c r="A370" s="3">
         <v>369</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="4">
+      <c r="A371" s="3">
         <v>370</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="4">
+      <c r="A372" s="3">
         <v>371</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="4">
+      <c r="A373" s="3">
         <v>372</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="4">
+      <c r="A374" s="3">
         <v>373</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="4">
+      <c r="A375" s="3">
         <v>374</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="4">
+      <c r="A376" s="3">
         <v>375</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="4">
+      <c r="A377" s="3">
         <v>376</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" s="4">
+      <c r="A378" s="3">
         <v>377</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="4">
+      <c r="A379" s="3">
         <v>378</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="4">
+      <c r="A380" s="3">
         <v>379</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="4">
+      <c r="A381" s="3">
         <v>380</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="4">
+      <c r="A382" s="3">
         <v>381</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="4">
+      <c r="A383" s="3">
         <v>382</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="4">
+      <c r="A384" s="3">
         <v>383</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" s="4">
+      <c r="A385" s="3">
         <v>384</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="4">
+      <c r="A386" s="3">
         <v>385</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="4">
+      <c r="A387" s="3">
         <v>386</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="4">
+      <c r="A388" s="3">
         <v>387</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="4">
+      <c r="A389" s="3">
         <v>388</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="4">
+      <c r="A390" s="3">
         <v>389</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="4">
+      <c r="A391" s="3">
         <v>390</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="4">
+      <c r="A392" s="3">
         <v>391</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" s="4">
+      <c r="A393" s="3">
         <v>392</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="4">
+      <c r="A394" s="3">
         <v>393</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="4">
+      <c r="A395" s="3">
         <v>394</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="4">
+      <c r="A396" s="3">
         <v>395</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="4">
+      <c r="A397" s="3">
         <v>396</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="4">
+      <c r="A398" s="3">
         <v>397</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" s="4">
+      <c r="A399" s="3">
         <v>398</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="4">
+      <c r="A400" s="3">
         <v>399</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="4">
+      <c r="A401" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="4">
+      <c r="A402" s="3">
         <v>401</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="4">
+      <c r="A403" s="3">
         <v>402</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="4">
+      <c r="A404" s="3">
         <v>403</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="4">
+      <c r="A405" s="3">
         <v>404</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" s="4">
+      <c r="A406" s="3">
         <v>405</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="4">
+      <c r="A407" s="3">
         <v>406</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="4">
+      <c r="A408" s="3">
         <v>407</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" s="4">
+      <c r="A409" s="3">
         <v>408</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="4">
+      <c r="A410" s="3">
         <v>409</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="4">
+      <c r="A411" s="3">
         <v>410</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="4">
+      <c r="A412" s="3">
         <v>411</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="4">
+      <c r="A413" s="3">
         <v>412</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="4">
+      <c r="A414" s="3">
         <v>413</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" s="4">
+      <c r="A415" s="3">
         <v>414</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="4">
+      <c r="A416" s="3">
         <v>415</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="4">
+      <c r="A417" s="3">
         <v>416</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" s="4">
+      <c r="A418" s="3">
         <v>417</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="4">
+      <c r="A419" s="3">
         <v>418</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" s="4">
+      <c r="A420" s="3">
         <v>419</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="4">
+      <c r="A421" s="3">
         <v>420</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="4">
+      <c r="A422" s="3">
         <v>421</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="4">
+      <c r="A423" s="3">
         <v>422</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="4">
+      <c r="A424" s="3">
         <v>423</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="4">
+      <c r="A425" s="3">
         <v>424</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="4">
+      <c r="A426" s="3">
         <v>425</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="4">
+      <c r="A427" s="3">
         <v>426</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="4">
+      <c r="A428" s="3">
         <v>427</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" s="4">
+      <c r="A429" s="3">
         <v>428</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="4">
+      <c r="A430" s="3">
         <v>429</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="4">
+      <c r="A431" s="3">
         <v>430</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="4">
+      <c r="A432" s="3">
         <v>431</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="4">
+      <c r="A433" s="3">
         <v>432</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="4">
+      <c r="A434" s="3">
         <v>433</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="4">
+      <c r="A435" s="3">
         <v>434</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="4">
+      <c r="A436" s="3">
         <v>435</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="4">
+      <c r="A437" s="3">
         <v>436</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="4">
+      <c r="A438" s="3">
         <v>437</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" s="4">
+      <c r="A439" s="3">
         <v>438</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="4">
+      <c r="A440" s="3">
         <v>439</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="4">
+      <c r="A441" s="3">
         <v>440</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="4">
+      <c r="A442" s="3">
         <v>441</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="4">
+      <c r="A443" s="3">
         <v>442</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="4">
+      <c r="A444" s="3">
         <v>443</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="4">
+      <c r="A445" s="3">
         <v>444</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="4">
+      <c r="A446" s="3">
         <v>445</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" s="4">
+      <c r="A447" s="3">
         <v>446</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="4">
+      <c r="A448" s="3">
         <v>447</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="4">
+      <c r="A449" s="3">
         <v>448</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="4">
+      <c r="A450" s="3">
         <v>449</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="4">
+      <c r="A451" s="3">
         <v>450</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="4">
+      <c r="A452" s="3">
         <v>451</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="4">
+      <c r="A453" s="3">
         <v>452</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="4">
+      <c r="A454" s="3">
         <v>453</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" s="4">
+      <c r="A455" s="3">
         <v>454</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="4">
+      <c r="A456" s="3">
         <v>455</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="4">
+      <c r="A457" s="3">
         <v>456</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="4">
+      <c r="A458" s="3">
         <v>457</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="4">
+      <c r="A459" s="3">
         <v>458</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="4">
+      <c r="A460" s="3">
         <v>459</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" s="4">
+      <c r="A461" s="3">
         <v>460</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="4">
+      <c r="A462" s="3">
         <v>461</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="4">
+      <c r="A463" s="3">
         <v>462</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="4">
+      <c r="A464" s="3">
         <v>463</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="4">
+      <c r="A465" s="3">
         <v>464</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="4">
+      <c r="A466" s="3">
         <v>465</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="4">
+      <c r="A467" s="3">
         <v>466</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" s="4">
+      <c r="A468" s="3">
         <v>467</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="4">
+      <c r="A469" s="3">
         <v>468</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="4">
+      <c r="A470" s="3">
         <v>469</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" s="4">
+      <c r="A471" s="3">
         <v>470</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="4">
+      <c r="A472" s="3">
         <v>471</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="4">
+      <c r="A473" s="3">
         <v>472</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="4">
+      <c r="A474" s="3">
         <v>473</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="4">
+      <c r="A475" s="3">
         <v>474</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="4">
+      <c r="A476" s="3">
         <v>475</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" s="4">
+      <c r="A477" s="3">
         <v>476</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="4">
+      <c r="A478" s="3">
         <v>477</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="4">
+      <c r="A479" s="3">
         <v>478</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" s="4">
+      <c r="A480" s="3">
         <v>479</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="4">
+      <c r="A481" s="3">
         <v>480</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" s="4">
+      <c r="A482" s="3">
         <v>481</v>
       </c>
     </row>

</xml_diff>